<commit_message>
Plan de Trabajo actualizado al 06/08/2019
</commit_message>
<xml_diff>
--- a/Plan de Trabajo.xlsx
+++ b/Plan de Trabajo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Evaluar resultados.</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Todo(a)s</t>
+  </si>
+  <si>
+    <t>Jerome</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +102,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,15 +124,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -401,7 +416,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,11 +473,14 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>